<commit_message>
PUB-2756 - Changes to First Tier Tribunal Hearing lists (#689)
* Text changes to list names - english and welsh

* Update tests

* Remove 'judges' and 'members' fields and add 'panel' field to wpafcc list

* Fix checkstyle and pmd issues

* Fix date format in test resource

* Update data models version

* Update Welsh translation for FTT Land Reg list

* Update data models version

* Update data models version

---------

Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/wpafcc-weekly-hearing-list/wpafccWeeklyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/wpafcc-weekly-hearing-list/wpafccWeeklyHearingList.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/wpafcc-weekly-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natasha.alker/Repos/pip/pip-data-management/src/integrationTest/resources/data/non-strategic/wpafcc-weekly-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D65CA66-6505-A94F-8370-B6224309019C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEB5D5E-54D5-5848-82D8-CC178C34E6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44260" yWindow="5480" windowWidth="23380" windowHeight="23640" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="-40900" yWindow="3280" windowWidth="35840" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -41,80 +25,77 @@
     <t>Date</t>
   </si>
   <si>
+    <t>Hearing time</t>
+  </si>
+  <si>
+    <t>Case reference number</t>
+  </si>
+  <si>
+    <t>Case name</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>Mode of hearing</t>
+  </si>
+  <si>
     <t>Venue</t>
   </si>
   <si>
+    <t>Additional information</t>
+  </si>
+  <si>
     <t>10am</t>
   </si>
   <si>
+    <t>1234.0</t>
+  </si>
+  <si>
+    <t>This is a case name</t>
+  </si>
+  <si>
+    <t>Judge A, Member A</t>
+  </si>
+  <si>
+    <t>Case Management Hearing</t>
+  </si>
+  <si>
+    <t>This is a venue name</t>
+  </si>
+  <si>
+    <t>This is additional information</t>
+  </si>
+  <si>
     <t>10:30am</t>
   </si>
   <si>
-    <t>Case reference number</t>
-  </si>
-  <si>
-    <t>Judge A</t>
-  </si>
-  <si>
-    <t>Member A</t>
-  </si>
-  <si>
-    <t>Judge B</t>
-  </si>
-  <si>
-    <t>Member B</t>
-  </si>
-  <si>
-    <t>This is a case name</t>
+    <t>1235.0</t>
   </si>
   <si>
     <t>This is another case name</t>
   </si>
   <si>
-    <t>Case Management Hearing</t>
+    <t>Judge B, Member B</t>
   </si>
   <si>
     <t>Oral Hearing</t>
   </si>
   <si>
-    <t>This is a venue name</t>
-  </si>
-  <si>
-    <t>This is additional information</t>
-  </si>
-  <si>
     <t>This is another additional information</t>
   </si>
   <si>
-    <t>Member(s)</t>
-  </si>
-  <si>
-    <t>Judge(s)</t>
-  </si>
-  <si>
-    <t>Case name</t>
-  </si>
-  <si>
-    <t>Mode of hearing</t>
-  </si>
-  <si>
-    <t>Additional information</t>
-  </si>
-  <si>
-    <t>Hearing time</t>
+    <t>12/16/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,10 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,109 +457,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2781C7-F977-7445-AEF2-132F18114BDA}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" customWidth="1"/>
-    <col min="7" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45642</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>45642</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>1234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>45642</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1235</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>